<commit_message>
AddEntry: checks if values are correct
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>C# Login/Registration first draft finished. Check of valid inputs.</t>
+  </si>
+  <si>
+    <t>Android Main GUI first draft; Pupil and Database class</t>
+  </si>
+  <si>
+    <t>C# Registration: checks if values are correct</t>
+  </si>
+  <si>
+    <t>Research MongoDB</t>
+  </si>
+  <si>
+    <t>Android Login bugs fixed</t>
+  </si>
+  <si>
+    <t>C# MainWindow with Menu finished; AddEntryWindow finished</t>
+  </si>
+  <si>
+    <t>Research MongoDB (not finished), Virtual Machine (Aphrodite? Not finished)</t>
+  </si>
+  <si>
+    <t>C# AddEntry: checks if values are correct</t>
+  </si>
+  <si>
+    <t>Android AddEntryWindow finished</t>
+  </si>
+  <si>
+    <t>Virtual Machine bug fixed. MongoDB locally installed; Table company created</t>
   </si>
 </sst>
 </file>
@@ -378,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +457,48 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43014</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43021</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43028</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
ListView Entries; Statis updated
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\5BHIFS\BSD\Praktikumsverwaltung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\5BHIFS\BSD\Praktikumsverwaltung\DesktopApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -71,20 +71,42 @@
     <t>Research MongoDB (not finished), Virtual Machine (Aphrodite? Not finished)</t>
   </si>
   <si>
-    <t>C# AddEntry: checks if values are correct</t>
-  </si>
-  <si>
-    <t>Android AddEntryWindow finished</t>
-  </si>
-  <si>
     <t>Virtual Machine bug fixed. MongoDB locally installed; Table company created</t>
+  </si>
+  <si>
+    <t>Android AddEntryWindow finished (90%)</t>
+  </si>
+  <si>
+    <r>
+      <t>C# AddEntry: checks if values are correct finished (100</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%)</t>
+    </r>
+  </si>
+  <si>
+    <t>Android AddEntryWindow Bug fixing (90%)</t>
+  </si>
+  <si>
+    <t>MongoDB in Virtual Machine installing (50%)</t>
+  </si>
+  <si>
+    <t>C# List of Entries (30%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +116,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -405,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +523,24 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43035</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
webbrowser and 2nd column listview dynamically (not finished)
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -96,28 +96,28 @@
     <t>Android AddEntryWindow Bug fixing (100%)</t>
   </si>
   <si>
-    <t>MongoDB in Virtual Machine installation finished  (100%)</t>
-  </si>
-  <si>
     <t>C# List of Entries and research google maps (location) (30%)</t>
   </si>
   <si>
-    <t>MongoDB research and first queries (30%)</t>
-  </si>
-  <si>
     <t>C# GoogleMaps in WebBrowser (50%)</t>
   </si>
   <si>
-    <t>Android research google maps (20%)</t>
-  </si>
-  <si>
-    <t>MongoDB installation aphrodite</t>
-  </si>
-  <si>
-    <t>Android dynamic creation of entries</t>
-  </si>
-  <si>
-    <t>C# GoogleMaps WebBrowser dynamically added</t>
+    <t>MongoDB locally adapted (80%).</t>
+  </si>
+  <si>
+    <t>MongoDB installation aphrodite "finished" (Mr. Oberlercher adapts aphrodite) (99%). Research and queries for the collections (40%)</t>
+  </si>
+  <si>
+    <t>MongoDB in Virtual Machine installation finished  (60%)</t>
+  </si>
+  <si>
+    <t>C# GoogleMaps WebBrowser dynamically added. 2nd column in progress (70%).</t>
+  </si>
+  <si>
+    <t>Android Research connection MongoDB with AndroidStudio (20%)</t>
+  </si>
+  <si>
+    <t>Android Creation of remaining activities, MongoDB jar added, connection in progress (40%)</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +555,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,10 +566,10 @@
         <v>43042</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -580,13 +580,13 @@
         <v>43049</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set intern ip address. status updated
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\5BHIFS\BSD\Praktikumsverwaltung\DesktopApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenz\Documents\5BHIFS\Praktikumsverwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>C# WebBrowser dynamically adding, still no reasonable way. Connection to MongoDB in order to get the entries: Filename too long. Probably change of directory needed (75%)</t>
+  </si>
+  <si>
+    <t>C# Displaying entries works (100%). Login works (100%).</t>
+  </si>
+  <si>
+    <t>MongoDB Inserts finished (100%)</t>
+  </si>
+  <si>
+    <t>Android get collection (documents) of mongoDB doesn't work. Null error (but connection is ok) (40%).</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +621,20 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43063</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
workaround (wrapper class) to display the location of the company. Multiple google maps work
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Android Get collection "works" (however, only in javafx =&gt; creating webservice in javafx to get data in android) (50%)</t>
+  </si>
+  <si>
+    <t>C# Admin Login: multiple columns in listview with buttons and images (to accept a new entry). Multiple Google Maps (Location of Company) through wrapper class. Both functions without mongoDB (100%)</t>
+  </si>
+  <si>
+    <t>WebService get collection pupil and entry (90%).</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +664,20 @@
         <v>34</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43077</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
status updated. New Entries Window which allows admin to accept or decline added entries
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>WebService get collection pupil and entry (90%).</t>
+  </si>
+  <si>
+    <t>WebService Login both Pupil and Teacher works, get all Entries works, join in mongoDB (helped Weiler) (50%)</t>
+  </si>
+  <si>
+    <t>WebService get collection pupil works (100%), added java Classes Pupil and Entry, join in MongoDB works in Console (50%)</t>
+  </si>
+  <si>
+    <t>WebService get collection pupil works (100%), adapted java classes, adapted Database methods (40%)</t>
   </si>
 </sst>
 </file>
@@ -486,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +687,20 @@
         <v>37</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43084</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
adminNote works. status updated
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -183,10 +183,19 @@
     <t>Android display of all entries (50%)</t>
   </si>
   <si>
-    <t>Research Web App Frameworks, decision: JSF, reading up in JSF (10%)</t>
-  </si>
-  <si>
     <t>C# Load admin gui elements in combination with webservice. (50%)  WebService bugfix Entries date (100%), however new bug: "no document validation"</t>
+  </si>
+  <si>
+    <t>Android display of all entries (100%). Communication of start- and enddate between two activities (30%)</t>
+  </si>
+  <si>
+    <t>C# LoadAdminGuiElements in combination with webservice (100%). Implementation of adminNote in all windows (40%)</t>
+  </si>
+  <si>
+    <t>Research Web App Frameworks, decision: JSF, reading up in JSF (10%), WebApp Login (100%), Display of all entries (100%), AddEntry (100%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading up in JSF (100%), Restore of MongoDB (it was empty) (100%), MongoDB adminNote added (100%) </t>
   </si>
 </sst>
 </file>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,10 +773,24 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43154</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="s">
-        <v>48</v>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login with active directory of school works. Admin note everywhere implemented except one window.
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t xml:space="preserve">Reading up in JSF (100%), Restore of MongoDB (it was empty) (100%), MongoDB adminNote added (100%) </t>
+  </si>
+  <si>
+    <t>WebApp  detailed display of entries and option to edit (detailed display 100%)(edit entry 50%)</t>
+  </si>
+  <si>
+    <t>C# Login with active directory of school (100%), Admin note (90%)</t>
+  </si>
+  <si>
+    <t>Android communication of start- and enddate between two activities (100%)</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,6 +802,20 @@
         <v>52</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43161</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
status updated, admin note
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Android communication of start- and enddate between two activities (100%)</t>
+  </si>
+  <si>
+    <t>WebApp edit entry (70%)</t>
+  </si>
+  <si>
+    <t>Android bugfix post methods -&gt; research, because they don't work (20%)</t>
+  </si>
+  <si>
+    <t>C# Admin note (100%). Login status bar does not work as it should work (20%)</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,6 +825,20 @@
         <v>53</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43168</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
admin note, status updated
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>C# Admin note (100%). Login status bar does not work as it should work (20%)</t>
+  </si>
+  <si>
+    <t>Android bugfix post methods -&gt; research (20%)</t>
+  </si>
+  <si>
+    <t>C# admin note communication between two windows fixed (80%)</t>
+  </si>
+  <si>
+    <t>WebApp bugfix (100%)</t>
   </si>
 </sst>
 </file>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +848,20 @@
         <v>56</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43175</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
layout slightly changed. status
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>WebApp bugfix (100%)</t>
+  </si>
+  <si>
+    <t>Android Layout (20%)</t>
+  </si>
+  <si>
+    <t>C# small layout adaption</t>
+  </si>
+  <si>
+    <t>WebApp layout (25%)</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,6 +871,20 @@
         <v>61</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43196</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
LdapAuthentication disabled because it does not work with mongodb architecture (no bson ids....)
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Sarkovic</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>WebApp layout (25%)</t>
+  </si>
+  <si>
+    <t>WebApp layout (50%). EditEntry (25%)</t>
+  </si>
+  <si>
+    <t>Android Layout (100%). Admin note (50%)</t>
+  </si>
+  <si>
+    <t>C# LdapAuthentication disabled, because it does not work with mongodb architecture (no bson ids…) (100%)</t>
   </si>
 </sst>
 </file>
@@ -567,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,6 +894,20 @@
         <v>64</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43203</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>